<commit_message>
MAJ DURIF après compilation
</commit_message>
<xml_diff>
--- a/mpsi2_TP.xlsx
+++ b/mpsi2_TP.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6980" yWindow="460" windowWidth="14380" windowHeight="14660"/>
+    <workbookView xWindow="6980" yWindow="460" windowWidth="14380" windowHeight="14200"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -582,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -804,7 +804,9 @@
       <c r="B18" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="2"/>
+      <c r="C18" s="2">
+        <v>1</v>
+      </c>
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -814,7 +816,9 @@
       <c r="B19" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C19" s="2"/>
+      <c r="C19" s="2">
+        <v>1</v>
+      </c>
       <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -824,7 +828,9 @@
       <c r="B20" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C20" s="2"/>
+      <c r="C20" s="2">
+        <v>1</v>
+      </c>
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -834,8 +840,12 @@
       <c r="B21" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="3"/>
+      <c r="C21" s="2">
+        <v>1</v>
+      </c>
+      <c r="D21" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
@@ -844,8 +854,12 @@
       <c r="B22" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+      <c r="C22" s="2">
+        <v>1</v>
+      </c>
+      <c r="D22" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
@@ -854,7 +868,9 @@
       <c r="B23" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="2"/>
+      <c r="C23" s="2">
+        <v>1</v>
+      </c>
       <c r="D23" s="3"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -864,7 +880,9 @@
       <c r="B24" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="2"/>
+      <c r="C24" s="2">
+        <v>1</v>
+      </c>
       <c r="D24" s="2"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -874,7 +892,9 @@
       <c r="B25" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="2"/>
+      <c r="C25" s="2">
+        <v>1</v>
+      </c>
       <c r="D25" s="3"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -884,7 +904,9 @@
       <c r="B26" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C26" s="2"/>
+      <c r="C26" s="2">
+        <v>1</v>
+      </c>
       <c r="D26" s="2"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -894,7 +916,9 @@
       <c r="B27" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="2"/>
+      <c r="C27" s="2">
+        <v>1</v>
+      </c>
       <c r="D27" s="3"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -904,7 +928,9 @@
       <c r="B28" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C28" s="2"/>
+      <c r="C28" s="2">
+        <v>1</v>
+      </c>
       <c r="D28" s="2"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -914,7 +940,9 @@
       <c r="B29" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="2"/>
+      <c r="C29" s="2">
+        <v>1</v>
+      </c>
       <c r="D29" s="3"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -924,7 +952,9 @@
       <c r="B30" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="2"/>
+      <c r="C30" s="2">
+        <v>1</v>
+      </c>
       <c r="D30" s="2"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -934,7 +964,9 @@
       <c r="B31" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C31" s="2"/>
+      <c r="C31" s="2">
+        <v>1</v>
+      </c>
       <c r="D31" s="3"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -944,7 +976,9 @@
       <c r="B32" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C32" s="2"/>
+      <c r="C32" s="2">
+        <v>1</v>
+      </c>
       <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -954,7 +988,9 @@
       <c r="B33" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C33" s="2"/>
+      <c r="C33" s="2">
+        <v>1</v>
+      </c>
       <c r="D33" s="3"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -1046,7 +1082,9 @@
       <c r="B42" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C42" s="2"/>
+      <c r="C42" s="2">
+        <v>1</v>
+      </c>
       <c r="D42" s="2"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -1096,7 +1134,9 @@
       <c r="B47" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C47" s="3"/>
+      <c r="C47" s="3">
+        <v>1</v>
+      </c>
       <c r="D47" s="3"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
ajout tp de sii
</commit_message>
<xml_diff>
--- a/mpsi2_TP.xlsx
+++ b/mpsi2_TP.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="65">
   <si>
     <t>Nom et prénom</t>
   </si>
@@ -220,6 +220,9 @@
   </si>
   <si>
     <t>TP13</t>
+  </si>
+  <si>
+    <t>DS7</t>
   </si>
 </sst>
 </file>
@@ -256,7 +259,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -279,15 +282,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -599,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -611,7 +626,7 @@
     <col min="3" max="5" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -642,8 +657,11 @@
       <c r="J1" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -673,7 +691,7 @@
       </c>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -697,7 +715,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -725,7 +743,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -755,7 +773,7 @@
       </c>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -783,7 +801,7 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -813,7 +831,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -845,7 +863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -877,7 +895,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -905,7 +923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -929,7 +947,7 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -959,7 +977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -987,7 +1005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -1015,7 +1033,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -1043,7 +1061,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
maj cours 4 bdd
</commit_message>
<xml_diff>
--- a/mpsi2_TP.xlsx
+++ b/mpsi2_TP.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="66">
   <si>
     <t>Nom et prénom</t>
   </si>
@@ -223,6 +223,9 @@
   </si>
   <si>
     <t>DS7</t>
+  </si>
+  <si>
+    <t>TP14</t>
   </si>
 </sst>
 </file>
@@ -614,9 +617,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K45"/>
+  <dimension ref="A1:L45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
@@ -626,7 +629,7 @@
     <col min="3" max="5" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -657,11 +660,14 @@
       <c r="J1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -690,8 +696,9 @@
         <v>1</v>
       </c>
       <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K2" s="2"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -714,8 +721,9 @@
       <c r="J3" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -742,8 +750,9 @@
       <c r="J4" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -772,8 +781,9 @@
         <v>1</v>
       </c>
       <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -800,8 +810,9 @@
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -830,8 +841,9 @@
       <c r="J7" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K7" s="3"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -862,8 +874,9 @@
       <c r="J8" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -894,8 +907,9 @@
       <c r="J9" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K9" s="3"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -922,8 +936,9 @@
       <c r="J10" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -946,8 +961,9 @@
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K11" s="3"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -976,8 +992,9 @@
       <c r="J12" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K12" s="2"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -1004,8 +1021,9 @@
       <c r="J13" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K13" s="3"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -1032,8 +1050,9 @@
       <c r="J14" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K14" s="2"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -1060,8 +1079,9 @@
       <c r="J15" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K15" s="3"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -1088,8 +1108,9 @@
       <c r="J16" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K16" s="2"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
@@ -1116,8 +1137,9 @@
       <c r="J17" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K17" s="3"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
@@ -1148,8 +1170,9 @@
       <c r="J18" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K18" s="2"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
@@ -1176,8 +1199,9 @@
       <c r="J19" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K19" s="3"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
@@ -1204,8 +1228,9 @@
       <c r="J20" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -1232,8 +1257,9 @@
       <c r="J21" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K21" s="3"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
@@ -1264,8 +1290,9 @@
       <c r="J22" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K22" s="2"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
@@ -1292,8 +1319,9 @@
       <c r="J23" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K23" s="3"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
@@ -1320,8 +1348,9 @@
       <c r="J24" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K24" s="2"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
@@ -1348,8 +1377,9 @@
       <c r="J25" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K25" s="3"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
@@ -1378,8 +1408,9 @@
         <v>1</v>
       </c>
       <c r="J26" s="2"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K26" s="2"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
@@ -1408,8 +1439,9 @@
         <v>1</v>
       </c>
       <c r="J27" s="3"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K27" s="3"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
@@ -1436,8 +1468,9 @@
       <c r="J28" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K28" s="2"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>28</v>
       </c>
@@ -1466,8 +1499,9 @@
         <v>1</v>
       </c>
       <c r="J29" s="3"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K29" s="3"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
@@ -1494,8 +1528,9 @@
       <c r="J30" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K30" s="2"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
@@ -1524,8 +1559,9 @@
         <v>1</v>
       </c>
       <c r="J31" s="2"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K31" s="2"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>31</v>
       </c>
@@ -1556,8 +1592,9 @@
       <c r="J32" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K32" s="3"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
@@ -1582,8 +1619,9 @@
       <c r="J33" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K33" s="2"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>33</v>
       </c>
@@ -1608,8 +1646,9 @@
       <c r="J34" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K34" s="3"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
@@ -1638,8 +1677,9 @@
       <c r="J35" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K35" s="2"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>35</v>
       </c>
@@ -1664,8 +1704,9 @@
       <c r="J36" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K36" s="3"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>36</v>
       </c>
@@ -1686,8 +1727,9 @@
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K37" s="2"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>38</v>
       </c>
@@ -1708,8 +1750,9 @@
       <c r="J38" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K38" s="2"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>39</v>
       </c>
@@ -1734,8 +1777,9 @@
       <c r="J39" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K39" s="2"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>40</v>
       </c>
@@ -1760,8 +1804,9 @@
       <c r="J40" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K40" s="3"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>41</v>
       </c>
@@ -1788,8 +1833,9 @@
         <v>1</v>
       </c>
       <c r="J41" s="2"/>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K41" s="2"/>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>42</v>
       </c>
@@ -1814,8 +1860,9 @@
       <c r="J42" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K42" s="3"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>43</v>
       </c>
@@ -1840,8 +1887,9 @@
       <c r="J43" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K43" s="2"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>44</v>
       </c>
@@ -1868,8 +1916,9 @@
       <c r="J44" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K44" s="3"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>45</v>
       </c>
@@ -1892,6 +1941,7 @@
       </c>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
+      <c r="K45" s="2"/>
     </row>
   </sheetData>
   <sortState ref="A3:J45">

</xml_diff>

<commit_message>
maj info 2 premier chapitre et TP
</commit_message>
<xml_diff>
--- a/mpsi2_TP.xlsx
+++ b/mpsi2_TP.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="860" windowWidth="25600" windowHeight="14220"/>
+    <workbookView xWindow="2380" yWindow="1560" windowWidth="19400" windowHeight="14220"/>
   </bookViews>
   <sheets>
     <sheet name="S2" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="68">
   <si>
     <t>Nom et prénom</t>
   </si>
@@ -226,6 +226,12 @@
   </si>
   <si>
     <t>TP14</t>
+  </si>
+  <si>
+    <t>DS9</t>
+  </si>
+  <si>
+    <t>Projet</t>
   </si>
 </sst>
 </file>
@@ -300,12 +306,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -617,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L46"/>
+  <dimension ref="A1:N46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="N50" sqref="N50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -629,7 +636,7 @@
     <col min="3" max="5" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -666,8 +673,14 @@
       <c r="L1" s="4" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M1" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -699,8 +712,14 @@
       <c r="K2" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2" s="5">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -724,8 +743,14 @@
         <v>1</v>
       </c>
       <c r="K3" s="3"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -755,8 +780,14 @@
       <c r="K4" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M4" s="5">
+        <v>1</v>
+      </c>
+      <c r="N4" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -788,8 +819,11 @@
       <c r="K5" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -817,8 +851,14 @@
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -850,8 +890,14 @@
       <c r="K7" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -885,8 +931,14 @@
       <c r="K8" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M8" s="5">
+        <v>1</v>
+      </c>
+      <c r="N8" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -920,8 +972,14 @@
       <c r="K9" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -951,8 +1009,14 @@
       <c r="K10" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M10" s="5">
+        <v>1</v>
+      </c>
+      <c r="N10" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -978,8 +1042,14 @@
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -1011,8 +1081,14 @@
       <c r="K12" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M12" s="5">
+        <v>1</v>
+      </c>
+      <c r="N12" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -1042,8 +1118,14 @@
       <c r="K13" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -1073,8 +1155,14 @@
       <c r="K14" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M14" s="5">
+        <v>1</v>
+      </c>
+      <c r="N14" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -1102,8 +1190,14 @@
         <v>1</v>
       </c>
       <c r="K15" s="3"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -1133,8 +1227,14 @@
       <c r="K16" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M16" s="5">
+        <v>1</v>
+      </c>
+      <c r="N16" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
@@ -1164,8 +1264,14 @@
       <c r="K17" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
@@ -1199,8 +1305,14 @@
       <c r="K18" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M18" s="5">
+        <v>1</v>
+      </c>
+      <c r="N18" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
@@ -1230,8 +1342,14 @@
       <c r="K19" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>19</v>
       </c>
@@ -1261,8 +1379,14 @@
       <c r="K20" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M20" s="5">
+        <v>1</v>
+      </c>
+      <c r="N20" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -1290,8 +1414,14 @@
         <v>1</v>
       </c>
       <c r="K21" s="3"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
@@ -1325,8 +1455,14 @@
       <c r="K22" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M22" s="5">
+        <v>1</v>
+      </c>
+      <c r="N22" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
@@ -1356,8 +1492,14 @@
       <c r="K23" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M23">
+        <v>1</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>23</v>
       </c>
@@ -1387,8 +1529,14 @@
       <c r="K24" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M24" s="5">
+        <v>1</v>
+      </c>
+      <c r="N24" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
@@ -1418,8 +1566,14 @@
       <c r="K25" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M25">
+        <v>1</v>
+      </c>
+      <c r="N25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>25</v>
       </c>
@@ -1449,8 +1603,14 @@
       </c>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M26" s="5">
+        <v>1</v>
+      </c>
+      <c r="N26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
@@ -1482,8 +1642,11 @@
       <c r="K27" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>27</v>
       </c>
@@ -1513,8 +1676,14 @@
       <c r="K28" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M28" s="5">
+        <v>1</v>
+      </c>
+      <c r="N28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>28</v>
       </c>
@@ -1544,8 +1713,14 @@
       </c>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M29">
+        <v>1</v>
+      </c>
+      <c r="N29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>29</v>
       </c>
@@ -1575,8 +1750,14 @@
       <c r="K30" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M30" s="5">
+        <v>1</v>
+      </c>
+      <c r="N30" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>30</v>
       </c>
@@ -1606,8 +1787,14 @@
       </c>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M31">
+        <v>1</v>
+      </c>
+      <c r="N31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>31</v>
       </c>
@@ -1641,8 +1828,14 @@
       <c r="K32" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M32">
+        <v>1</v>
+      </c>
+      <c r="N32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>32</v>
       </c>
@@ -1668,8 +1861,14 @@
         <v>1</v>
       </c>
       <c r="K33" s="2"/>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M33" s="5">
+        <v>1</v>
+      </c>
+      <c r="N33" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>33</v>
       </c>
@@ -1697,8 +1896,14 @@
       <c r="K34" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M34">
+        <v>1</v>
+      </c>
+      <c r="N34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>34</v>
       </c>
@@ -1730,8 +1935,14 @@
       <c r="K35" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M35" s="5">
+        <v>1</v>
+      </c>
+      <c r="N35" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>35</v>
       </c>
@@ -1759,8 +1970,14 @@
       <c r="K36" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M36">
+        <v>1</v>
+      </c>
+      <c r="N36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>36</v>
       </c>
@@ -1784,8 +2001,14 @@
       <c r="K37" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M37">
+        <v>1</v>
+      </c>
+      <c r="N37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>38</v>
       </c>
@@ -1809,8 +2032,14 @@
       <c r="K38" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M38" s="5">
+        <v>1</v>
+      </c>
+      <c r="N38" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>39</v>
       </c>
@@ -1836,8 +2065,14 @@
         <v>1</v>
       </c>
       <c r="K39" s="2"/>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M39" s="5">
+        <v>1</v>
+      </c>
+      <c r="N39" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>40</v>
       </c>
@@ -1863,8 +2098,11 @@
         <v>1</v>
       </c>
       <c r="K40" s="3"/>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="N40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>41</v>
       </c>
@@ -1894,8 +2132,14 @@
       <c r="K41" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M41" s="5">
+        <v>1</v>
+      </c>
+      <c r="N41" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>42</v>
       </c>
@@ -1923,8 +2167,14 @@
       <c r="K42" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M42">
+        <v>1</v>
+      </c>
+      <c r="N42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>43</v>
       </c>
@@ -1952,8 +2202,14 @@
       <c r="K43" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M43" s="5">
+        <v>1</v>
+      </c>
+      <c r="N43" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>44</v>
       </c>
@@ -1983,8 +2239,14 @@
       <c r="K44" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M44">
+        <v>1</v>
+      </c>
+      <c r="N44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>45</v>
       </c>
@@ -2009,10 +2271,14 @@
       <c r="J45" s="2"/>
       <c r="K45" s="2"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="I46">
         <f>SUM(I2:I45)</f>
         <v>41</v>
+      </c>
+      <c r="M46">
+        <f>SUM(M2:M45)</f>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>